<commit_message>
Adjustment, primarily to fix figure Q21-3 when prepped together
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_parameters.xlsx
+++ b/inst/extdata/plot_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0415858C-AAEF-B143-B614-1FDCD6B59D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63BFE7F-B668-3343-A373-85D41D77C55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="21140" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="labels" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="603">
   <si>
     <t>Variable</t>
   </si>
@@ -1811,13 +1811,34 @@
   </si>
   <si>
     <t>No Preferred Language</t>
+  </si>
+  <si>
+    <t>SHEET</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>This sheet contains information that helps us make concise labels for plots.</t>
+  </si>
+  <si>
+    <t>logic</t>
+  </si>
+  <si>
+    <t>This sheet contains information that provides the logic for plotting functions in cdrs.</t>
+  </si>
+  <si>
+    <t>palettes</t>
+  </si>
+  <si>
+    <t>This sheet contains information on different color palette combinations. It shares the pal_id column with SHEET logic.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1957,6 +1978,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2300,11 +2327,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2682,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" topLeftCell="C77" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3466,6 +3494,9 @@
       <c r="A57" t="s">
         <v>162</v>
       </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
       <c r="C57" t="s">
         <v>21</v>
       </c>
@@ -4064,6 +4095,7 @@
       <c r="B101" t="s">
         <v>280</v>
       </c>
+      <c r="C101" s="2"/>
       <c r="D101" t="s">
         <v>124</v>
       </c>
@@ -4114,6 +4146,9 @@
       <c r="C105" t="s">
         <v>289</v>
       </c>
+      <c r="D105" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -4125,6 +4160,9 @@
       <c r="C106" t="s">
         <v>292</v>
       </c>
+      <c r="D106" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -4134,6 +4172,9 @@
         <v>294</v>
       </c>
       <c r="C107" t="s">
+        <v>295</v>
+      </c>
+      <c r="D107" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4863,8 +4904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126:C141"/>
+    <sheetView topLeftCell="A64" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5815,7 +5856,7 @@
         <v>183</v>
       </c>
       <c r="B86" t="s">
-        <v>465</v>
+        <v>565</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -7867,10 +7908,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7891,43 +7932,43 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>544</v>
+        <v>596</v>
+      </c>
+      <c r="B2" t="s">
+        <v>597</v>
       </c>
       <c r="C2" t="s">
-        <v>545</v>
+        <v>598</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>544</v>
+        <v>596</v>
       </c>
       <c r="B3" t="s">
-        <v>444</v>
+        <v>599</v>
       </c>
       <c r="C3" t="s">
-        <v>546</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>544</v>
+        <v>596</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>601</v>
       </c>
       <c r="C4" t="s">
-        <v>547</v>
+        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>544</v>
       </c>
-      <c r="B5" t="s">
-        <v>437</v>
-      </c>
       <c r="C5" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -7935,10 +7976,10 @@
         <v>544</v>
       </c>
       <c r="B6" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="C6" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -7946,10 +7987,10 @@
         <v>544</v>
       </c>
       <c r="B7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C7" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -7957,10 +7998,10 @@
         <v>544</v>
       </c>
       <c r="B8" t="s">
-        <v>465</v>
+        <v>437</v>
       </c>
       <c r="C8" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -7968,42 +8009,75 @@
         <v>544</v>
       </c>
       <c r="B9" t="s">
-        <v>565</v>
+        <v>436</v>
       </c>
       <c r="C9" t="s">
-        <v>566</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
       <c r="B10" t="s">
-        <v>567</v>
+        <v>438</v>
       </c>
       <c r="C10" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>544</v>
+      </c>
+      <c r="B11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C11" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>544</v>
+      </c>
+      <c r="B12" t="s">
+        <v>565</v>
+      </c>
+      <c r="C12" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>559</v>
+      </c>
+      <c r="B13" t="s">
+        <v>567</v>
+      </c>
+      <c r="C13" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>573</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>567</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>579</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>567</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>580</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incremented version to reflect progress on maps (but still unfinished)
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_parameters.xlsx
+++ b/inst/extdata/plot_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4B2267-8E68-6146-BD70-F371CEC0CFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE598738-CAFF-E341-8CE3-BF52847928CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="21140" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C77" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4904,8 +4904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView topLeftCell="A221" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B220" sqref="B220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
corrected labels for Q7 and 24, which somehow got mixed up.
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_parameters.xlsx
+++ b/inst/extdata/plot_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE598738-CAFF-E341-8CE3-BF52847928CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB942A-6B01-9647-9C89-B258D1BC3FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="21140" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3344,10 +3344,10 @@
         <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3358,10 +3358,10 @@
         <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3372,10 +3372,10 @@
         <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3386,10 +3386,10 @@
         <v>126</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -3400,10 +3400,10 @@
         <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -3414,10 +3414,10 @@
         <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -3428,10 +3428,10 @@
         <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -3442,10 +3442,10 @@
         <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -3456,10 +3456,10 @@
         <v>126</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D54" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3470,10 +3470,10 @@
         <v>126</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -3484,10 +3484,10 @@
         <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -4214,10 +4214,10 @@
         <v>297</v>
       </c>
       <c r="C110" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="D110" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -4228,10 +4228,10 @@
         <v>297</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D111" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -4242,10 +4242,10 @@
         <v>297</v>
       </c>
       <c r="C112" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="D112" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4256,10 +4256,10 @@
         <v>297</v>
       </c>
       <c r="C113" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="D113" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -4270,10 +4270,10 @@
         <v>297</v>
       </c>
       <c r="C114" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="D114" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -4284,10 +4284,10 @@
         <v>297</v>
       </c>
       <c r="C115" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="D115" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -4298,10 +4298,10 @@
         <v>297</v>
       </c>
       <c r="C116" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="D116" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -4312,10 +4312,10 @@
         <v>297</v>
       </c>
       <c r="C117" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="D117" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -4326,10 +4326,10 @@
         <v>297</v>
       </c>
       <c r="C118" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="D118" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -4340,10 +4340,10 @@
         <v>297</v>
       </c>
       <c r="C119" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="D119" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -4354,10 +4354,10 @@
         <v>297</v>
       </c>
       <c r="C120" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="D120" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -4368,10 +4368,10 @@
         <v>297</v>
       </c>
       <c r="C121" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="D121" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -4382,10 +4382,10 @@
         <v>297</v>
       </c>
       <c r="C122" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="D122" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -4396,10 +4396,10 @@
         <v>297</v>
       </c>
       <c r="C123" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="D123" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added label info for Q1a
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_parameters.xlsx
+++ b/inst/extdata/plot_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0336ADA-3EDD-BC4D-9047-8BDF7E3D9228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0A2A38-4830-004C-BD9F-0D7A2ACCBB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="702">
   <si>
     <t>Variable</t>
   </si>
@@ -2123,6 +2123,12 @@
   </si>
   <si>
     <t>Resident owned</t>
+  </si>
+  <si>
+    <t>okabegr</t>
+  </si>
+  <si>
+    <t>Years in the Delta</t>
   </si>
 </sst>
 </file>
@@ -3037,9 +3043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G178" sqref="G178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,7 +3268,7 @@
         <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>701</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>40</v>
@@ -5894,8 +5900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6189,6 +6195,9 @@
       <c r="B34" t="s">
         <v>429</v>
       </c>
+      <c r="C34" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -8665,10 +8674,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3678AB9-5160-2F47-AB46-A977D8766B75}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8889,6 +8898,23 @@
       </c>
       <c r="D14" t="s">
         <v>583</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>429</v>
+      </c>
+      <c r="B15" t="s">
+        <v>700</v>
+      </c>
+      <c r="C15" t="s">
+        <v>551</v>
+      </c>
+      <c r="D15" t="s">
+        <v>550</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted ordinal/diverging plots. Stacked bar plots no longer show a label unless label_form is specified to "qid", plot_parameters actually has a label. For instance, compare Q34 and Q13a: Q34 has no label, but Q13a does have a label.
</commit_message>
<xml_diff>
--- a/inst/extdata/plot_parameters.xlsx
+++ b/inst/extdata/plot_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/cdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0A2A38-4830-004C-BD9F-0D7A2ACCBB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11F8DC0-6282-1B47-AC10-624E5EF39BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="704">
   <si>
     <t>Variable</t>
   </si>
@@ -2129,6 +2129,12 @@
   </si>
   <si>
     <t>Years in the Delta</t>
+  </si>
+  <si>
+    <t>Willing to answer supplemental questions</t>
+  </si>
+  <si>
+    <t>Supplemental questions?</t>
   </si>
 </sst>
 </file>
@@ -3043,9 +3049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4037,12 +4043,6 @@
       <c r="D65" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -4952,6 +4952,12 @@
       </c>
       <c r="D125" s="1" t="s">
         <v>341</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -5900,8 +5906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E246"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A80" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>